<commit_message>
REFACTOR: Removing unwanted suites
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>EnableScheduler</t>
-  </si>
-  <si>
-    <t>NextAndBackButtons</t>
-  </si>
-  <si>
-    <t>Unwritten</t>
   </si>
   <si>
     <t>ProgressBar</t>
@@ -187,16 +181,20 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -214,20 +212,16 @@
     </dxf>
     <dxf>
       <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FF66FF66"/>
         </patternFill>
       </fill>
     </dxf>
@@ -546,7 +540,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,14 +569,14 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$2:A37)</f>
-        <v>5</v>
+        <f>COUNTA($A$2:A36)</f>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$2:D36,"Ready to Write")+COUNTIF($D$2:D36,"Outdated")</f>
+        <f>COUNTIF($D$2:D35,"Ready to Write")+COUNTIF($D$2:D35,"Outdated")</f>
         <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -610,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="6">
-        <f>COUNTIF($D$2:D36,"Automated")+COUNTIF($D$2:D36,"Finished")</f>
+        <f>COUNTIF($D$2:D35,"Automated")+COUNTIF($D$2:D35,"Finished")</f>
         <v>2</v>
       </c>
     </row>
@@ -625,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -638,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
@@ -647,47 +641,35 @@
         <v>8</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$2:C36)</f>
+        <f>SUM($C$2:C35)</f>
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$2:B36)</f>
+        <f>SUM($B$2:B35)</f>
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
@@ -711,26 +693,26 @@
   <sortState ref="A2:E8">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D50">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="notContainsBlanks" dxfId="7" priority="9" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>

</xml_diff>

<commit_message>
FUNCTIONALITY: EnableScheduler - Finished testing. RequiredFields - Finished testing. SchedulingCreateValidation - Noted broken test cases. Custodian - Wrote a keyword.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -63,13 +63,7 @@
     <t>Suited to Manual</t>
   </si>
   <si>
-    <t>Visuals</t>
-  </si>
-  <si>
     <t>RequiredFields</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -540,7 +534,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +578,7 @@
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -605,7 +599,7 @@
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D$2:D35,"Automated")+COUNTIF($D$2:D35,"Finished")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -613,13 +607,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -647,7 +641,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -658,15 +652,12 @@
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B35)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,7 +666,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.78787878787878785</v>
+        <v>0.81818181818181823</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Step1Fields - Updated and corrected a few test cases and tested a few more. NextAndBackButtonStates - Corrected the documentation.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Title</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Percentage Automated:</t>
   </si>
   <si>
-    <t>CreateStep1Fields</t>
-  </si>
-  <si>
     <t>EnableScheduler</t>
   </si>
   <si>
@@ -64,6 +61,12 @@
   </si>
   <si>
     <t>RequiredFields</t>
+  </si>
+  <si>
+    <t>Step1Fields</t>
+  </si>
+  <si>
+    <t>One test case is untested and waiting on TBH143</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,16 +586,19 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1">
         <v>20</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -604,7 +610,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>5</v>
@@ -620,7 +626,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -629,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
@@ -641,7 +647,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
@@ -657,7 +663,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B35)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -666,7 +672,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.81818181818181823</v>
+        <v>0.84848484848484851</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Updated the workspace name variables.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -537,7 +537,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,19 +586,16 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -610,32 +607,32 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
@@ -647,16 +644,19 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>9</v>
@@ -687,7 +687,7 @@
     <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="A2:E8">
+  <sortState ref="A2:E5">
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D2:D49">

</xml_diff>

<commit_message>
FUNCTIONALITY: Big update. IntegrationPointKeywords - Wrote a new keyword and fixed a different keyword. RequiredFields - Updated the existing automation and wrote two new test cases. Step1Fields - Fixed a bunch of timing errors. SchedulingRequiredFields - Added the colon to some field names and fixed a timing error. ConnectionValidation - Finished testing. Step2Fields - Updated the existing automation and wrote a new test case.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -537,7 +537,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,10 +626,10 @@
         <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -639,7 +639,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$2:C35)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B$2:B35)</f>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -672,7 +672,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.84848484848484851</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
REFACTOR: Added tests for Email Notification
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -534,7 +534,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -644,10 +644,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -657,7 +657,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.86842105263157898</v>
+        <v>0.87179487179487181</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: EmailNotification tests Updated JobHistory
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Step1Fields</t>
+  </si>
+  <si>
+    <t>EmailNotification</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -158,7 +164,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -534,7 +674,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +704,7 @@
       </c>
       <c r="E1" s="4">
         <f>COUNTA($A:$A) - 1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
@@ -604,50 +744,53 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -661,12 +804,24 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.87179487179487181</v>
+        <v>0.82926829268292679</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -684,32 +839,60 @@
   <sortState ref="A2:E5">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D49">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="D2 D4:D49">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+  <conditionalFormatting sqref="D1:D2 D4:D1048576">
+    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(D3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FUNCTIONALITY: Prepped for Crucible submission.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -228,6 +228,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -282,13 +289,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -674,7 +674,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,16 +723,19 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -744,19 +747,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
@@ -839,60 +839,60 @@
   <sortState ref="A2:E5">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="D2 D4:D49">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="17" stopIfTrue="1">
+  <conditionalFormatting sqref="D3:D49">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="25" stopIfTrue="1">
+      <formula>LEN(TRIM(D3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1 D3:D1048576">
+    <cfRule type="containsText" dxfId="14" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D2 D4:D1048576">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(D3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor test case updates
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/Step1/_Test_Suite_Statistics.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Title</t>
   </si>
@@ -74,7 +74,7 @@
     <t>EmailNotification</t>
   </si>
   <si>
-    <t>Email</t>
+    <t>Ready to Write</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,14 +652,14 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -673,9 +673,6 @@
         <v>2</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">

</xml_diff>